<commit_message>
Fix data error where envelope energy use was greater than 0
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SYCEU/Start Year Components Energy Use.xlsx
+++ b/InputData/bldgs/SYCEU/Start Year Components Energy Use.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\bldgs\SYCEU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB5D545-E42A-48DE-B3AE-7C2A836C03C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9584DE1-A133-4EFC-8333-CE03550B7AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23881,7 +23881,7 @@
       <selection activeCell="M41" sqref="M41"/>
       <selection pane="topRight" activeCell="M41" sqref="M41"/>
       <selection pane="bottomLeft" activeCell="M41" sqref="M41"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2:G11"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -23957,7 +23957,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="14">
         <f>'2020 Calculations'!K96</f>
@@ -23985,7 +23985,7 @@
         <v>11164069695813.242</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E4" s="14">
         <f>'2020 Calculations'!K97</f>
@@ -24013,7 +24013,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E5" s="14">
         <f>'2020 Calculations'!K98</f>
@@ -24041,7 +24041,7 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E6" s="14">
         <f>'2020 Calculations'!K99</f>
@@ -24069,7 +24069,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E7" s="14">
         <f>'2020 Calculations'!K100</f>
@@ -24097,7 +24097,7 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E8" s="14">
         <f>'2020 Calculations'!K101</f>
@@ -24125,7 +24125,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E9" s="14">
         <f>'2020 Calculations'!K102</f>
@@ -24153,7 +24153,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E10" s="14">
         <f>'2020 Calculations'!K103</f>
@@ -24181,7 +24181,7 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E11" s="14">
         <f>'2020 Calculations'!K104</f>
@@ -70370,7 +70370,7 @@
         <v>1789100000000000</v>
       </c>
       <c r="T136" s="60">
-        <f t="shared" ref="O136:Y137" si="94">INDEX(Table5_22,MATCH($H136,Table5_A_22,0),MATCH(T$133,Table5_1_22,0))*quadrillion</f>
+        <f t="shared" ref="O136:T137" si="94">INDEX(Table5_22,MATCH($H136,Table5_A_22,0),MATCH(T$133,Table5_1_22,0))*quadrillion</f>
         <v>1789100000000000</v>
       </c>
       <c r="U136" s="60">

</xml_diff>